<commit_message>
added pocket to arm
</commit_message>
<xml_diff>
--- a/Torque Calculations.xlsx
+++ b/Torque Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deli\OneDrive - Eastside Preparatory School\FTC\8103-power-play\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FDF120-1E0E-4C33-86B4-9B06E09450AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745313B7-CE04-4448-B1B6-259578F42FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{0D04A8BF-92C0-4572-8E9A-212B8C5F260D}"/>
+    <workbookView xWindow="-28920" yWindow="-270" windowWidth="29040" windowHeight="17640" xr2:uid="{0D04A8BF-92C0-4572-8E9A-212B8C5F260D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +578,7 @@
         <v>96</v>
       </c>
       <c r="F2">
-        <f>B2*E2</f>
+        <f t="shared" ref="F2:F7" si="0">B2*E2</f>
         <v>576</v>
       </c>
       <c r="H2">
@@ -593,11 +593,11 @@
         <v>1.7381571947350152</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2">
         <f>J2*K2</f>
-        <v>1.7381571947350152</v>
+        <v>3.4763143894700304</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -618,7 +618,7 @@
         <v>60.620351957448314</v>
       </c>
       <c r="F3">
-        <f>B3*E3</f>
+        <f t="shared" si="0"/>
         <v>242.48140782979326</v>
       </c>
     </row>
@@ -633,7 +633,7 @@
         <v>3.3</v>
       </c>
       <c r="F4">
-        <f>B4*E4</f>
+        <f t="shared" si="0"/>
         <v>26.4</v>
       </c>
     </row>
@@ -655,7 +655,7 @@
         <v>58.822668163081268</v>
       </c>
       <c r="F5">
-        <f>B5*E5</f>
+        <f t="shared" si="0"/>
         <v>117.64533632616254</v>
       </c>
     </row>
@@ -670,7 +670,7 @@
         <v>69</v>
       </c>
       <c r="F6">
-        <f>B6*E6</f>
+        <f t="shared" si="0"/>
         <v>138</v>
       </c>
     </row>
@@ -685,7 +685,7 @@
         <v>64</v>
       </c>
       <c r="F7">
-        <f>B7*E7</f>
+        <f t="shared" si="0"/>
         <v>192</v>
       </c>
     </row>
@@ -700,7 +700,7 @@
         <v>7.8</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F34" si="0">B8*E8</f>
+        <f t="shared" ref="F8:F34" si="1">B8*E8</f>
         <v>31.2</v>
       </c>
     </row>
@@ -722,7 +722,7 @@
         <v>55.714527826700852</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>111.4290556534017</v>
       </c>
     </row>
@@ -737,7 +737,7 @@
         <v>14</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -752,7 +752,7 @@
         <v>3.5</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -767,7 +767,7 @@
         <v>3</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
@@ -782,7 +782,7 @@
         <v>3.4</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.8</v>
       </c>
     </row>
@@ -797,7 +797,7 @@
         <v>7.3</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.6</v>
       </c>
     </row>
@@ -819,7 +819,7 @@
         <v>13.312833013846925</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.312833013846925</v>
       </c>
     </row>
@@ -841,7 +841,7 @@
         <v>8.5242809559051906</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.048561911810381</v>
       </c>
     </row>
@@ -856,7 +856,7 @@
         <v>5.4</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.200000000000003</v>
       </c>
     </row>
@@ -871,7 +871,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.1999999999999993</v>
       </c>
     </row>
@@ -886,7 +886,7 @@
         <v>21</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -901,7 +901,7 @@
         <v>62</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
     </row>
@@ -916,7 +916,7 @@
         <v>11</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
@@ -931,7 +931,7 @@
         <v>8.5</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
     </row>
@@ -946,7 +946,7 @@
         <v>1.9</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8</v>
       </c>
     </row>
@@ -961,7 +961,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1399999999999999</v>
       </c>
     </row>
@@ -976,7 +976,7 @@
         <v>0.16</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
     </row>
@@ -991,7 +991,7 @@
         <v>0.32</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
         <v>1.3</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
         <v>1.5</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -1036,7 +1036,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1051,7 +1051,7 @@
         <v>2.4</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.6</v>
       </c>
     </row>
@@ -1066,25 +1066,25 @@
         <v>0.78</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.12</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>